<commit_message>
templates for changed tables regenerated
</commit_message>
<xml_diff>
--- a/StagingTemplates/Staging.OrganizationType.xlsx
+++ b/StagingTemplates/Staging.OrganizationType.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="25050" windowHeight="11175"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="18885" windowHeight="10245"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>For internal use only. Do not fill in or change</t>
   </si>
@@ -35,7 +35,13 @@
     <t>BusinessKey</t>
   </si>
   <si>
+    <t>Code</t>
+  </si>
+  <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
 </sst>
 </file>
@@ -364,7 +370,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet36"/>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -373,12 +379,12 @@
     <col min="1" max="1" width="41" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -387,6 +393,12 @@
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>